<commit_message>
[2] Use OpenCSV for reading PBL.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
-    <sheet name="PBL" sheetId="1" r:id="rId1"/>
+    <sheet name="PBL2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -86,6 +86,9 @@
     <t>Akzeptanzkriterien:
 - aus dem CSV laden, im PBL anzeigen, im Burnup anzeigen und persistieren.
 - Status: Todo, In Progress, Done, Canceled</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -920,7 +923,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[PBL] Updated estimate of ID 1.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -923,7 +923,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
[PBL] - [2] fertiggestellt. - Neues PBI für Editieren und Speichern von Sprint Daten. - [5] "Import von Sprint Daten" als nächstes PBI ausgewählt.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -33,10 +33,6 @@
   <si>
     <t>Akzeptanzkriterien:
 - Id, Title, Summary und Estimate</t>
-  </si>
-  <si>
-    <t>Akzeptanzkriterien:
-- Name, Anfangsdatum, Enddatum, geplante Kapazität, geplanter Aufwand, tatsächliche Kapazität, Aufwand DONE</t>
   </si>
   <si>
     <t>Als PO möchte ich Sprint-Daten aus einer CSV-Datei importieren und tabellarisch anzeigen können.</t>
@@ -89,6 +85,20 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Sprintname, Anfangsdatum, Enddatum, geplante Kapazität, geplanter Aufwand, tatsächliche Kapazität, Aufwand Done</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich Sprint-Daten editieren, speichern und wieder laden können.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Alle Felder aus [5] können editiert werden.
+- Sprints können gelöscht werden.
+- Neue Sprints können hinzugefügt werden.
+- Die Persistierung erfolgt als XML-Datei.</t>
   </si>
 </sst>
 </file>
@@ -920,15 +930,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
   </cols>
@@ -947,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -955,16 +965,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -981,106 +991,123 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
+      <c r="E9" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[5] Refactoring des CSV-Importers als Vorbereitung für den Import von Sprints.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Id</t>
   </si>
@@ -99,6 +99,18 @@
 - Sprints können gelöscht werden.
 - Neue Sprints können hinzugefügt werden.
 - Die Persistierung erfolgt als XML-Datei.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 1, Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -930,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,9 +953,10 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,8 +972,11 @@
       <c r="E1" t="s">
         <v>17</v>
       </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -976,8 +992,11 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -993,8 +1012,11 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1010,8 +1032,11 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1022,13 +1047,16 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1045,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1059,7 +1087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1076,7 +1104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1093,7 +1121,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
[PBL] - [5] "Import von Sprint Daten" fertiggestellt.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -945,7 +945,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[6] Einlesen und Anzeigen des Status eines PBIs.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Id</t>
   </si>
@@ -77,11 +77,6 @@
   </si>
   <si>
     <t>Todo</t>
-  </si>
-  <si>
-    <t>Akzeptanzkriterien:
-- aus dem CSV laden, im PBL anzeigen, im Burnup anzeigen und persistieren.
-- Status: Todo, In Progress, Done, Canceled</t>
   </si>
   <si>
     <t>Done</t>
@@ -111,6 +106,22 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- aus dem CSV laden, im PBL anzeigen
+- Status: Todo, In Progress, Done, Canceled</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Zur Berechnung wird die normierte Geschwindigkeit verwendet:
+-- Abgeschlossener Sprint: EffortDone/CapacityDone
+-- Laufender Sprint: EffortForecast/CapacityForecast
+- Diese wird mit der Kapazität des Sprints multipliziert.
+- Der Forecast ergibt sich aus den  normierten Geschwindigkeiten aller vorherigen Sprints multipliziert mit der Forecast-Kapazität des Sprints.</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich den Effort-Forecast für jeden Sprint sehen können.</t>
   </si>
 </sst>
 </file>
@@ -942,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -990,10 +1001,10 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1010,10 +1021,10 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1024,19 +1035,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1044,27 +1055,27 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1072,69 +1083,89 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
         <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PBL] - [10] Berechnung und Anzeige des Effort-Forecasts fertiggestellt.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -122,6 +122,26 @@
   </si>
   <si>
     <t>Als PO möchte ich den Effort-Forecast für jeden Sprint sehen können.</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich den akkumulieren Effort-Forecast bis zu jedem Sprint sehen können.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Die Geschwindigkeiten werden wie bei [10] berechnet.
+- Der akkumulierte Forecast ergibt sich aus dem akkumulierten Forecast des vorherigen Sprints plus dem
+Effort-Forecast dieses Sprints</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich für alle PBIs einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkritrien:
+- Hierzu werden die akkumulierten Effort-Forecast aus [11] verwendet.
+- Der Sprint-Forecast wird im PBL dargestellt</t>
   </si>
 </sst>
 </file>
@@ -953,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,91 +1101,131 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PBL] Story [11] fertig.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -121,27 +121,28 @@
 - Der Forecast ergibt sich aus den  normierten Geschwindigkeiten aller vorherigen Sprints multipliziert mit der Forecast-Kapazität des Sprints.</t>
   </si>
   <si>
-    <t>Als PO möchte ich den Effort-Forecast für jeden Sprint sehen können.</t>
-  </si>
-  <si>
-    <t>Als PO möchte ich den akkumulieren Effort-Forecast bis zu jedem Sprint sehen können.</t>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich für alle PBIs einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkritrien:
+- Hierzu werden die akkumulierten Effort-Forecast aus [11] verwendet.
+- Der Sprint-Forecast wird im PBL dargestellt</t>
   </si>
   <si>
     <t>Akzeptanzkriterien:
 - Die Geschwindigkeiten werden wie bei [10] berechnet.
 - Der akkumulierte Forecast ergibt sich aus dem akkumulierten Forecast des vorherigen Sprints plus dem
-Effort-Forecast dieses Sprints</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Als PO möchte ich für alle PBIs einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
-  </si>
-  <si>
-    <t>Akzeptanzkritrien:
-- Hierzu werden die akkumulierten Effort-Forecast aus [11] verwendet.
-- Der Sprint-Forecast wird im PBL dargestellt</t>
+Progress-Forecast dieses Sprints
+- Für abgeschlossene Sprints wird kein Progress-Forecast angezeigt.</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich den akkumulieren Progress-Forecast bis zu jedem Sprint sehen können.</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich den Progress-Forecast für jeden Sprint sehen können.</t>
   </si>
 </sst>
 </file>
@@ -975,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -1107,24 +1108,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1132,10 +1133,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1144,7 +1145,7 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[12] Berechnung der akkumulierten Aufwandschätzung bis zur Fertigstellung jedes PBIs.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -124,9 +124,6 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Als PO möchte ich für alle PBIs einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
-  </si>
-  <si>
     <t>Akzeptanzkritrien:
 - Hierzu werden die akkumulierten Effort-Forecast aus [11] verwendet.
 - Der Sprint-Forecast wird im PBL dargestellt</t>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Als PO möchte ich den Progress-Forecast für jeden Sprint sehen können.</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich für jedes PBI einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -1113,10 +1113,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1133,10 +1133,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D8">
         <v>2</v>

</xml_diff>

<commit_message>
[PBL] Planning Sprint 4.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="PBL2" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Als PO möchte ich für jedes PBI einen Forecast bis zu welchem Sprint dieses fertiggestellt wird.</t>
+  </si>
+  <si>
+    <t>Sprint 3, Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1148,7 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[PBL] Neue Zusätzliches PBI für Sprint 4.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
-    <sheet name="PBL2" sheetId="1" r:id="rId1"/>
+    <sheet name="PBL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Sprint 3, Sprint 4</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich Releases durch die Angabe der ID eines PBIs definieren können. Für diese Releases werden die Forecasts berechnet, bis zu welchen Sprint diese fertiggestellt sind.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriteren:
+- Die Releases werden in einer Taballe auf einem neuen Tab dargestellt.
+- Die Releases können editiert und abgespeichert werden.
+- Es wird angezeigt, wenn es kein PBI mit dieser ID gibt.</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -977,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,95 +1157,116 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
         <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[15] Use the same column names as the Jira export.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,18 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Summary</t>
-  </si>
-  <si>
-    <t>Estimate</t>
   </si>
   <si>
     <t>Als PO möchte ich PBIs aus einer CSV-Datei importieren und als PBL in einer Tabelle anzeigen können</t>
@@ -71,9 +62,6 @@
   </si>
   <si>
     <t>Als PO möchte ich Trendlinien mit minimaler und maximaler Geschwindigkeit im Burnup anzeigen lassen können</t>
-  </si>
-  <si>
-    <t>State</t>
   </si>
   <si>
     <t>Todo</t>
@@ -151,13 +139,34 @@
     <t>Als PO möchte ich Releases durch die Angabe der ID eines PBIs definieren können. Für diese Releases werden die Forecasts berechnet, bis zu welchen Sprint diese fertiggestellt sind.</t>
   </si>
   <si>
-    <t>Akzeptanzkriteren:
-- Die Releases werden in einer Taballe auf einem neuen Tab dargestellt.
-- Die Releases können editiert und abgespeichert werden.
-- Es wird angezeigt, wenn es kein PBI mit dieser ID gibt.</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
+    <t xml:space="preserve">Akzeptanzkriteren:
+- Die Releases werden in einer Tabelle auf einem neuen Tab dargestellt.
+</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich Releases erfassen, editieren und abspeichern können.</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich einen PBL-Export aus Jira als CSV einlesen können</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Die PBIs werden sortiert nach Sprint-Nummer und dann nach Rank</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -989,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,22 +1014,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1028,19 +1037,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1048,19 +1057,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1068,19 +1077,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1088,19 +1097,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
@@ -1108,19 +1117,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1128,19 +1137,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1148,121 +1157,155 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>18</v>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "[15] Use the same column names as the Jira export."
This reverts commit 91bde6585b86fe2ab66c92acfff14f3ba7def7d4.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Estimate</t>
   </si>
   <si>
     <t>Als PO möchte ich PBIs aus einer CSV-Datei importieren und als PBL in einer Tabelle anzeigen können</t>
@@ -62,6 +71,9 @@
   </si>
   <si>
     <t>Als PO möchte ich Trendlinien mit minimaler und maximaler Geschwindigkeit im Burnup anzeigen lassen können</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
   <si>
     <t>Todo</t>
@@ -139,34 +151,13 @@
     <t>Als PO möchte ich Releases durch die Angabe der ID eines PBIs definieren können. Für diese Releases werden die Forecasts berechnet, bis zu welchen Sprint diese fertiggestellt sind.</t>
   </si>
   <si>
-    <t xml:space="preserve">Akzeptanzkriteren:
-- Die Releases werden in einer Tabelle auf einem neuen Tab dargestellt.
-</t>
-  </si>
-  <si>
-    <t>Als PO möchte ich Releases erfassen, editieren und abspeichern können.</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Als PO möchte ich einen PBL-Export aus Jira als CSV einlesen können</t>
-  </si>
-  <si>
-    <t>Akzeptanzkriterien:
-- Die PBIs werden sortiert nach Sprint-Nummer und dann nach Rank</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Story Points</t>
-  </si>
-  <si>
-    <t>Status</t>
+    <t>Akzeptanzkriteren:
+- Die Releases werden in einer Taballe auf einem neuen Tab dargestellt.
+- Die Releases können editiert und abgespeichert werden.
+- Es wird angezeigt, wenn es kein PBI mit dieser ID gibt.</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -998,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,22 +1005,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1037,19 +1028,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1057,19 +1048,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1077,19 +1068,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1097,19 +1088,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
@@ -1117,19 +1108,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1137,19 +1128,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1157,155 +1148,121 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "[15] Use the same column names as the Jira export.""
This reverts commit 9575b8c693945dfb672cfc164ffac49269dd60f8.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,18 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Summary</t>
-  </si>
-  <si>
-    <t>Estimate</t>
   </si>
   <si>
     <t>Als PO möchte ich PBIs aus einer CSV-Datei importieren und als PBL in einer Tabelle anzeigen können</t>
@@ -71,9 +62,6 @@
   </si>
   <si>
     <t>Als PO möchte ich Trendlinien mit minimaler und maximaler Geschwindigkeit im Burnup anzeigen lassen können</t>
-  </si>
-  <si>
-    <t>State</t>
   </si>
   <si>
     <t>Todo</t>
@@ -151,13 +139,34 @@
     <t>Als PO möchte ich Releases durch die Angabe der ID eines PBIs definieren können. Für diese Releases werden die Forecasts berechnet, bis zu welchen Sprint diese fertiggestellt sind.</t>
   </si>
   <si>
-    <t>Akzeptanzkriteren:
-- Die Releases werden in einer Taballe auf einem neuen Tab dargestellt.
-- Die Releases können editiert und abgespeichert werden.
-- Es wird angezeigt, wenn es kein PBI mit dieser ID gibt.</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
+    <t xml:space="preserve">Akzeptanzkriteren:
+- Die Releases werden in einer Tabelle auf einem neuen Tab dargestellt.
+</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich Releases erfassen, editieren und abspeichern können.</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich einen PBL-Export aus Jira als CSV einlesen können</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+- Die PBIs werden sortiert nach Sprint-Nummer und dann nach Rank</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -989,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,22 +1014,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1028,19 +1037,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1048,19 +1057,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1068,19 +1077,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1088,19 +1097,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
@@ -1108,19 +1117,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1128,19 +1137,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1148,121 +1157,155 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>18</v>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[15] Sort PBIs by sprint and then by rank.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Summary</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Rank</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1015,7 @@
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1031,8 +1034,11 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1051,8 +1057,11 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1071,8 +1080,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1091,8 +1103,11 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1111,8 +1126,11 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1131,8 +1149,11 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -1151,8 +1172,11 @@
       <c r="F7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -1171,8 +1195,11 @@
       <c r="F8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -1191,8 +1218,11 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -1211,8 +1241,11 @@
       <c r="F10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1228,8 +1261,11 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1242,8 +1278,11 @@
       <c r="E12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1259,8 +1298,11 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1276,8 +1318,11 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1293,8 +1338,11 @@
       <c r="E15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1306,6 +1354,9 @@
       </c>
       <c r="E16" t="s">
         <v>14</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[15] Use Resolution column to determine state of PBIs.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -64,12 +64,6 @@
     <t>Als PO möchte ich Trendlinien mit minimaler und maximaler Geschwindigkeit im Burnup anzeigen lassen können</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Akzeptanzkriterien:
 - Sprintname, Anfangsdatum, Enddatum, geplante Kapazität, geplanter Aufwand, tatsächliche Kapazität, Aufwand Done</t>
   </si>
@@ -166,10 +160,16 @@
     <t>Story Points</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,30 +1012,31 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1052,10 +1053,10 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1075,10 +1076,10 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1092,16 +1093,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1115,16 +1116,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -1135,19 +1136,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1158,19 +1159,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -1181,19 +1182,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -1204,19 +1205,19 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -1227,19 +1228,19 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -1259,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -1276,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -1287,16 +1288,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -1316,7 +1317,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -1336,7 +1337,7 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G15">
         <v>14</v>
@@ -1347,13 +1348,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G16">
         <v>15</v>

</xml_diff>

<commit_message>
[PBL] Added another PBI to Sprint 5. New PBI for adding and deleting sprints.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Summary</t>
   </si>
@@ -170,6 +170,13 @@
   </si>
   <si>
     <t>Unresolved</t>
+  </si>
+  <si>
+    <t>Als PO möchte ich Sprints hinzufügen und löschen können.</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien:
+Die Sprints werden nach aufsteigendem Start-Datum sortiert</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -1263,7 +1270,7 @@
         <v>42</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1280,7 +1287,7 @@
         <v>42</v>
       </c>
       <c r="G12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -1299,8 +1306,11 @@
       <c r="E13" t="s">
         <v>42</v>
       </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
       <c r="G13">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1358,6 +1368,26 @@
       </c>
       <c r="G16">
         <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UI Test improvements to Backlog.
</commit_message>
<xml_diff>
--- a/ProductBacklog/PBL.xlsx
+++ b/ProductBacklog/PBL.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="PBL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Summary</t>
   </si>
@@ -177,6 +178,21 @@
   <si>
     <t>Akzeptanzkriterien:
 Die Sprints werden nach aufsteigendem Start-Datum sortiert</t>
+  </si>
+  <si>
+    <t>Als Entwickler möchte ich die UI-Tests debuggen können, ohne dass diese unterbrochen werden</t>
+  </si>
+  <si>
+    <t>Akzeptanzkriterien: Die UI-Tests brechen nicht mehr ab, wenn die Maus bewegt wird,.</t>
+  </si>
+  <si>
+    <t>Als Entwickler möchte ich, dass die UI-Tests in einer angemessenen Geschwindigkeit laufen</t>
+  </si>
+  <si>
+    <t>Akzeptannzkriterien: Die UI-Tests laufen wesentlich schneller als zuvor</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -668,54 +684,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -764,7 +783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -799,7 +818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,13 +1027,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.85546875" bestFit="1" customWidth="1"/>
@@ -1390,6 +1409,46 @@
         <v>16</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>